<commit_message>
first completed run with rotation constraints; testing will begin in earnest
</commit_message>
<xml_diff>
--- a/data/Crop Rotation Sample Template - 2 crops and 2 fields.xlsx
+++ b/data/Crop Rotation Sample Template - 2 crops and 2 fields.xlsx
@@ -16,6 +16,9 @@
     <sheet name="Crops" sheetId="1" r:id="rId2"/>
     <sheet name="Demand" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Crops!$A$2:$X$46</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -961,10 +964,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:X46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="I41" sqref="I41"/>
@@ -1098,7 +1102,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -1148,7 +1152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>92</v>
       </c>
@@ -1251,7 +1255,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -1303,7 +1307,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>100</v>
       </c>
@@ -1357,7 +1361,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>99</v>
       </c>
@@ -1409,7 +1413,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
@@ -1465,7 +1469,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>96</v>
       </c>
@@ -1514,7 +1518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>94</v>
       </c>
@@ -1565,7 +1569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -1614,7 +1618,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
@@ -1668,7 +1672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1720,7 +1724,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -1772,7 +1776,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
@@ -1822,7 +1826,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:24" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" s="5" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>43</v>
       </c>
@@ -1876,7 +1880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:24" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" s="5" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>50</v>
       </c>
@@ -1928,7 +1932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:24" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" s="5" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
@@ -1980,7 +1984,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:24" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" s="5" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>48</v>
       </c>
@@ -2032,7 +2036,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
@@ -2086,7 +2090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
@@ -2140,7 +2144,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>56</v>
       </c>
@@ -2194,7 +2198,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>53</v>
       </c>
@@ -2246,7 +2250,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
@@ -2298,7 +2302,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>58</v>
       </c>
@@ -2350,7 +2354,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>60</v>
       </c>
@@ -2402,7 +2406,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>62</v>
       </c>
@@ -2454,7 +2458,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>63</v>
       </c>
@@ -2506,7 +2510,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>93</v>
       </c>
@@ -2557,7 +2561,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>66</v>
       </c>
@@ -2613,7 +2617,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>75</v>
       </c>
@@ -2664,7 +2668,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>76</v>
       </c>
@@ -2713,7 +2717,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>67</v>
       </c>
@@ -2762,7 +2766,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>68</v>
       </c>
@@ -2820,7 +2824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>70</v>
       </c>
@@ -2876,7 +2880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>71</v>
       </c>
@@ -2932,7 +2936,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>72</v>
       </c>
@@ -2988,7 +2992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>74</v>
       </c>
@@ -3037,7 +3041,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>90</v>
       </c>
@@ -3088,7 +3092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>77</v>
       </c>
@@ -3138,7 +3142,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>80</v>
       </c>
@@ -3235,7 +3239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -3285,7 +3289,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>87</v>
       </c>
@@ -3326,7 +3330,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>89</v>
       </c>
@@ -3378,6 +3382,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:X46">
+    <filterColumn colId="23">
+      <filters>
+        <filter val="Y"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="K1:V1"/>
   </mergeCells>

</xml_diff>